<commit_message>
Updating graphs to be same structure (color, size, format, etc)
</commit_message>
<xml_diff>
--- a/CCK8-Transfection_Plots/20231211_CCK8-Transfection_DIPLibrary_reducedserum.xlsx
+++ b/CCK8-Transfection_Plots/20231211_CCK8-Transfection_DIPLibrary_reducedserum.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Documents - Aryelle’s MacBook Air/Kumar-Biomaterials-Lab/CCK8_Transfection_Plots/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Documents - Aryelle’s MacBook Air/Kumar-Biomaterials-Lab/CCK8-Transfection_Plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993F0550-F3A4-614B-A725-7C51978AB3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698A3140-2668-CF42-B5C0-229AAF567715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="660" windowWidth="24420" windowHeight="15980" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="660" windowWidth="24420" windowHeight="15980" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="DIPPolyplexesCalcs2" sheetId="6" r:id="rId7"/>
     <sheet name="PolymerOnly" sheetId="3" r:id="rId8"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="MethodPointer1">1759294816</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="107">
   <si>
     <t>Software Version</t>
   </si>
@@ -354,6 +355,18 @@
   </si>
   <si>
     <t>Untreated</t>
+  </si>
+  <si>
+    <t>Polymer</t>
+  </si>
+  <si>
+    <t>N/P Ratio</t>
+  </si>
+  <si>
+    <t>Stdev</t>
+  </si>
+  <si>
+    <t>STD_Viability</t>
   </si>
 </sst>
 </file>
@@ -2665,6 +2678,526 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99341371-646B-0D4F-8882-B5BDB1610B63}">
+  <dimension ref="A1:F1048576"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="D2">
+        <v>5.773502691896258E-3</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>4.8562229493959439</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.19000000000000003</v>
+      </c>
+      <c r="D3">
+        <v>4.5825756949558372E-2</v>
+      </c>
+      <c r="E3">
+        <v>73.344947735191653</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>61.753333333333337</v>
+      </c>
+      <c r="D4">
+        <v>4.9677895822320517</v>
+      </c>
+      <c r="E4">
+        <v>91.114982578397218</v>
+      </c>
+      <c r="F4">
+        <v>2.1194294530655773</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>58.93</v>
+      </c>
+      <c r="D5">
+        <v>2.3766362784406025</v>
+      </c>
+      <c r="E5">
+        <v>58.536585365853668</v>
+      </c>
+      <c r="F5">
+        <v>9.9226695929604247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>50.883333333333333</v>
+      </c>
+      <c r="D7">
+        <v>3.1989425336090886</v>
+      </c>
+      <c r="E7">
+        <v>30.139372822299649</v>
+      </c>
+      <c r="F7">
+        <v>5.6479320827342647</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8">
+        <v>7.5</v>
+      </c>
+      <c r="C8">
+        <v>57.650000000000006</v>
+      </c>
+      <c r="D8">
+        <v>0.30805843601499044</v>
+      </c>
+      <c r="E8">
+        <v>24.321329639889193</v>
+      </c>
+      <c r="F8">
+        <v>3.8634467305509022</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0.08</v>
+      </c>
+      <c r="D11">
+        <v>7.2111025509279794E-2</v>
+      </c>
+      <c r="E11">
+        <v>90.011614401858296</v>
+      </c>
+      <c r="F11">
+        <v>4.3565619822325221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>7.5</v>
+      </c>
+      <c r="C12">
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="D12">
+        <v>7.5055534994651382E-2</v>
+      </c>
+      <c r="E12">
+        <v>93.074792243767305</v>
+      </c>
+      <c r="F12">
+        <v>3.4704619974217956</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>48.733333333333327</v>
+      </c>
+      <c r="D15">
+        <v>1.4189197769195159</v>
+      </c>
+      <c r="E15">
+        <v>34.204413472706158</v>
+      </c>
+      <c r="F15">
+        <v>1.2359928370379072</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16">
+        <v>7.5</v>
+      </c>
+      <c r="C16">
+        <v>52.126666666666665</v>
+      </c>
+      <c r="D16">
+        <v>6.658328118479527E-2</v>
+      </c>
+      <c r="E16">
+        <v>24.321329639889196</v>
+      </c>
+      <c r="F16">
+        <v>3.066170438121147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>33.660000000000004</v>
+      </c>
+      <c r="D19">
+        <v>0.87109126961530092</v>
+      </c>
+      <c r="E19">
+        <v>31.30193905817174</v>
+      </c>
+      <c r="F19">
+        <v>6.1772232087607311</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20">
+        <v>7.5</v>
+      </c>
+      <c r="C20">
+        <v>44.22</v>
+      </c>
+      <c r="D20">
+        <v>0.59101607423148805</v>
+      </c>
+      <c r="E20">
+        <v>27.922437673130197</v>
+      </c>
+      <c r="F20">
+        <v>2.912146615169291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>24.756666666666671</v>
+      </c>
+      <c r="D23">
+        <v>0.49074772881118062</v>
+      </c>
+      <c r="E23">
+        <v>53.019390581717452</v>
+      </c>
+      <c r="F23">
+        <v>2.912146615169291</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24">
+        <v>7.5</v>
+      </c>
+      <c r="C24">
+        <v>32.884999999999998</v>
+      </c>
+      <c r="D24">
+        <v>0.5868986283848332</v>
+      </c>
+      <c r="E24">
+        <v>39.00277008310249</v>
+      </c>
+      <c r="F24">
+        <v>3.0661704381211563</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048576" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1048576" s="41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1389271-5B62-5E46-B1D0-300481CC9DBA}">
   <dimension ref="B2:O29"/>
@@ -4457,7 +4990,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E10"/>
+      <selection activeCell="B6" sqref="B6:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5048,7 +5581,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E10"/>
+      <selection activeCell="B6" sqref="B6:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6263,7 +6796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5B6B2A-22BB-234A-99B7-8736E7874F4B}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>

</xml_diff>